<commit_message>
AutoCommit_17 июня 2024 г. 11:42:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ТерВер.xlsx
+++ b/2ИСИП-122_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>2ИСИП-122: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>изм</t>
+  </si>
+  <si>
+    <t>выаы</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -570,12 +573,12 @@
     <col min="3" max="11" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -608,7 +611,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -635,7 +638,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -675,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -715,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -755,7 +758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -795,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -835,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -875,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -915,7 +918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -955,7 +958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -995,7 +998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1123,16 +1126,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E16" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G16" s="4">
         <v>5</v>
@@ -1141,18 +1144,21 @@
         <v>5</v>
       </c>
       <c r="I16" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J16" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="M16" s="7">
         <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 22:24:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ТерВер.xlsx
+++ b/2ИСИП-122_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>2ИСИП-122: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -139,15 +139,6 @@
   </si>
   <si>
     <t>лаб_1</t>
-  </si>
-  <si>
-    <t>изм</t>
-  </si>
-  <si>
-    <t>выаы</t>
-  </si>
-  <si>
-    <t>ВЫАЫВАЫ</t>
   </si>
 </sst>
 </file>
@@ -563,13 +554,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -579,12 +570,12 @@
     <col min="3" max="11" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -617,7 +608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -639,15 +630,11 @@
       <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="M3" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -687,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -727,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -767,7 +754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -807,7 +794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -847,7 +834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -887,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -927,7 +914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -967,7 +954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1007,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1047,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1087,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1127,7 +1114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1166,11 +1153,8 @@
       <c r="M16" s="7">
         <v>5</v>
       </c>
-      <c r="O16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1210,7 +1194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1250,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1289,11 +1273,8 @@
       <c r="M19" s="7">
         <v>4</v>
       </c>
-      <c r="O19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1332,11 +1313,8 @@
       <c r="M20" s="7">
         <v>4</v>
       </c>
-      <c r="O20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1376,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1416,7 +1394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1456,7 +1434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1496,7 +1474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1536,7 +1514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1576,7 +1554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1615,11 +1593,8 @@
       <c r="M27" s="7">
         <v>4</v>
       </c>
-      <c r="O27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1659,7 +1634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1699,7 +1674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1739,7 +1714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1779,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_26 июня 2024 г. 12:11:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ТерВер.xlsx
+++ b/2ИСИП-122_ТерВер.xlsx
@@ -557,13 +557,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomRight" activeCell="R4" sqref="R4:U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -573,12 +573,12 @@
     <col min="3" max="11" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -614,7 +614,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -643,8 +643,20 @@
       <c r="M3" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -690,8 +702,24 @@
         <f>O4-M4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <f>IF(R$3=$M4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:U19" si="0">IF(S$3=$M4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -724,7 +752,7 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5">
-        <f t="shared" ref="L5:L32" si="0">SUM(C5:J5)</f>
+        <f t="shared" ref="L5:L32" si="1">SUM(C5:J5)</f>
         <v>40</v>
       </c>
       <c r="M5" s="6">
@@ -734,11 +762,27 @@
         <v>5</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:P32" si="1">O5-M5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="P5:P32" si="2">O5-M5</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:U32" si="3">IF(R$3=$M5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -771,7 +815,7 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M6" s="6">
@@ -781,11 +825,27 @@
         <v>5</v>
       </c>
       <c r="P6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -818,7 +878,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="M7" s="6">
@@ -828,11 +888,27 @@
         <v>4</v>
       </c>
       <c r="P7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -865,7 +941,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="M8" s="7">
@@ -875,11 +951,27 @@
         <v>4</v>
       </c>
       <c r="P8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -912,7 +1004,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="M9" s="6">
@@ -922,11 +1014,27 @@
         <v>3</v>
       </c>
       <c r="P9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -959,7 +1067,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M10" s="6">
@@ -969,11 +1077,27 @@
         <v>5</v>
       </c>
       <c r="P10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1006,7 +1130,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M11" s="6">
@@ -1016,11 +1140,27 @@
         <v>5</v>
       </c>
       <c r="P11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1053,7 +1193,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M12" s="6">
@@ -1063,11 +1203,27 @@
         <v>5</v>
       </c>
       <c r="P12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1100,7 +1256,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="M13" s="7">
@@ -1110,11 +1266,27 @@
         <v>4</v>
       </c>
       <c r="P13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1147,7 +1319,7 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="M14" s="7">
@@ -1157,11 +1329,27 @@
         <v>4</v>
       </c>
       <c r="P14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1194,7 +1382,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M15" s="7">
@@ -1204,11 +1392,27 @@
         <v>5</v>
       </c>
       <c r="P15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1241,7 +1445,7 @@
       </c>
       <c r="K16" s="2"/>
       <c r="L16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M16" s="7">
@@ -1251,11 +1455,27 @@
         <v>5</v>
       </c>
       <c r="P16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1288,7 +1508,7 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M17" s="6">
@@ -1298,11 +1518,27 @@
         <v>5</v>
       </c>
       <c r="P17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1335,7 +1571,7 @@
       </c>
       <c r="K18" s="2"/>
       <c r="L18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M18" s="6">
@@ -1345,11 +1581,27 @@
         <v>5</v>
       </c>
       <c r="P18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1382,7 +1634,7 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="M19" s="7">
@@ -1392,11 +1644,27 @@
         <v>4</v>
       </c>
       <c r="P19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1429,7 +1697,7 @@
       </c>
       <c r="K20" s="2"/>
       <c r="L20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="M20" s="7">
@@ -1439,11 +1707,27 @@
         <v>4</v>
       </c>
       <c r="P20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1476,7 +1760,7 @@
       </c>
       <c r="K21" s="2"/>
       <c r="L21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M21" s="6">
@@ -1486,11 +1770,27 @@
         <v>5</v>
       </c>
       <c r="P21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1523,7 +1823,7 @@
       </c>
       <c r="K22" s="2"/>
       <c r="L22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="M22" s="7">
@@ -1533,11 +1833,27 @@
         <v>4</v>
       </c>
       <c r="P22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1570,7 +1886,7 @@
       </c>
       <c r="K23" s="2"/>
       <c r="L23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M23" s="6">
@@ -1580,11 +1896,27 @@
         <v>5</v>
       </c>
       <c r="P23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1617,7 +1949,7 @@
       </c>
       <c r="K24" s="2"/>
       <c r="L24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="M24" s="7">
@@ -1627,11 +1959,27 @@
         <v>5</v>
       </c>
       <c r="P24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1664,7 +2012,7 @@
       </c>
       <c r="K25" s="2"/>
       <c r="L25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M25" s="6">
@@ -1674,11 +2022,27 @@
         <v>4</v>
       </c>
       <c r="P25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1721,11 +2085,27 @@
         <v>5</v>
       </c>
       <c r="P26">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1758,7 +2138,7 @@
       </c>
       <c r="K27" s="2"/>
       <c r="L27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="M27" s="7">
@@ -1768,11 +2148,27 @@
         <v>3</v>
       </c>
       <c r="P27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1805,7 +2201,7 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M28" s="6">
@@ -1815,11 +2211,27 @@
         <v>4</v>
       </c>
       <c r="P28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1852,7 +2264,7 @@
       </c>
       <c r="K29" s="2"/>
       <c r="L29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M29" s="6">
@@ -1862,11 +2274,27 @@
         <v>5</v>
       </c>
       <c r="P29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1899,7 +2327,7 @@
       </c>
       <c r="K30" s="2"/>
       <c r="L30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="M30" s="7">
@@ -1909,11 +2337,27 @@
         <v>5</v>
       </c>
       <c r="P30">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1946,7 +2390,7 @@
       </c>
       <c r="K31" s="2"/>
       <c r="L31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M31" s="6">
@@ -1956,11 +2400,27 @@
         <v>4</v>
       </c>
       <c r="P31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1993,7 +2453,7 @@
       </c>
       <c r="K32" s="2"/>
       <c r="L32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="M32" s="7">
@@ -2003,8 +2463,24 @@
         <v>5</v>
       </c>
       <c r="P32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="3:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
@@ -2021,6 +2497,18 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="C4:J32 M21:M32 M4 M7:M9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L32">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2032,7 +2520,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L32">
+  <conditionalFormatting sqref="M4:M32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2044,7 +2532,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M32">
+  <conditionalFormatting sqref="R4:U32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_26 июня 2024 г. 12:15:10_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_ТерВер.xlsx
+++ b/2ИСИП-122_ТерВер.xlsx
@@ -557,13 +557,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="H16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R4" sqref="R4:U32"/>
+      <selection pane="bottomRight" activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2483,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:21" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2493,6 +2493,38 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>2</v>
+      </c>
+      <c r="S34">
+        <v>3</v>
+      </c>
+      <c r="T34">
+        <v>4</v>
+      </c>
+      <c r="U34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <f>SUM(R4:R32)</f>
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <f t="shared" ref="S36:U36" si="4">SUM(S4:S32)</f>
+        <v>2</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>